<commit_message>
5 May 2025 Update
</commit_message>
<xml_diff>
--- a/Translations.xlsx
+++ b/Translations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12481" uniqueCount="3017">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12842" uniqueCount="3114">
   <si>
     <t>2025-04-17T23-47-44-458Z</t>
   </si>
@@ -9026,6 +9026,297 @@
   </si>
   <si>
     <t>Honourable mention: Cupra Leon Sportstourer269k 0-100 4.9s</t>
+  </si>
+  <si>
+    <t>2025-05-31T14-30-05-013Z</t>
+  </si>
+  <si>
+    <t>inputs/sgcmchat_messages191_part3.csv</t>
+  </si>
+  <si>
+    <t>i will probs go down next month when i receive the car</t>
+  </si>
+  <si>
+    <t>i will probably go down next month when i have received the car</t>
+  </si>
+  <si>
+    <t>so far i got one recc to try there</t>
+  </si>
+  <si>
+    <t>so far i have gotten one recc to try it there</t>
+  </si>
+  <si>
+    <t>i'll prolly visit them this week</t>
+  </si>
+  <si>
+    <t>All for sale collection at cnk tmr!</t>
+  </si>
+  <si>
+    <t>Pm for prices  buy more  more discount</t>
+  </si>
+  <si>
+    <t>Pm for the prices. if you buy more, you get greater discount</t>
+  </si>
+  <si>
+    <t>This too is for sale pm for price!</t>
+  </si>
+  <si>
+    <t>This, too, is for sale. PM for the price!</t>
+  </si>
+  <si>
+    <t>Anyone going for coffee at Dempsey tomorrow morning?</t>
+  </si>
+  <si>
+    <t>Is anyone going for coffee at Dempsey Road tomorrow morning?</t>
+  </si>
+  <si>
+    <t>Bro your clip cant even reach 0:01</t>
+  </si>
+  <si>
+    <t>Bro, your clip cant even reach 0:01</t>
+  </si>
+  <si>
+    <t>anyone at dempsey can update the turnout</t>
+  </si>
+  <si>
+    <t>is there anyone at dempsey road now that can update us regarding the turnout</t>
+  </si>
+  <si>
+    <t>a lot of cars no space to park</t>
+  </si>
+  <si>
+    <t>a lot of cars around, there is no available space to park the car</t>
+  </si>
+  <si>
+    <t>It’s better now. A few groups left.</t>
+  </si>
+  <si>
+    <t>It’s better now. A few groups have left.</t>
+  </si>
+  <si>
+    <t>chat i saw the medusa going past opposite demsey bus stop</t>
+  </si>
+  <si>
+    <t>chat, i saw the medusa going past the bus stop that is across demsey road.</t>
+  </si>
+  <si>
+    <t>camera battery pack died and after i left this thing pulls up my timing is impeccable</t>
+  </si>
+  <si>
+    <t>camera battery pack died and after i left, this thing pulls up. My timing is impeccable</t>
+  </si>
+  <si>
+    <t>Anyone manage to take photos or videos of the Alfas?</t>
+  </si>
+  <si>
+    <t>Anyone managed to take photos or videos of the Alfas?</t>
+  </si>
+  <si>
+    <t>not a 1.6 convert for once 🤣</t>
+  </si>
+  <si>
+    <t>not a 1.6 conversion for once 🤣</t>
+  </si>
+  <si>
+    <t>Can’t tell the diff between r8s and s2000s</t>
+  </si>
+  <si>
+    <t>one is 1992 more than the other</t>
+  </si>
+  <si>
+    <t>Almost couldn't get a parking lot</t>
+  </si>
+  <si>
+    <t>I could barely get a parking lot</t>
+  </si>
+  <si>
+    <t>My aunty gave me consent form to do so</t>
+  </si>
+  <si>
+    <t>My aunty gave me consent to do so</t>
+  </si>
+  <si>
+    <t>ohh so u play wif  ur aunty ah</t>
+  </si>
+  <si>
+    <t>ohh so u play with ur auntie</t>
+  </si>
+  <si>
+    <t>i only play bacarat with her on cny</t>
+  </si>
+  <si>
+    <t>anyone here knows why the car wont start even after wiring</t>
+  </si>
+  <si>
+    <t>anyone on here knows why the car wont start even after wiring it?</t>
+  </si>
+  <si>
+    <t>maybe both car battery flat liao (jk)</t>
+  </si>
+  <si>
+    <t>maybe both car batteries are already flat (jk)</t>
+  </si>
+  <si>
+    <t>have you tested if the battery is dead?</t>
+  </si>
+  <si>
+    <t>have you tested to check if the battery is dead?</t>
+  </si>
+  <si>
+    <t>are you sure the jumper cables are connected properly?</t>
+  </si>
+  <si>
+    <t>are you sure the jumper cables are properly connected?</t>
+  </si>
+  <si>
+    <t>pos to pos neg to neg</t>
+  </si>
+  <si>
+    <t>pos to pos, neg to neg</t>
+  </si>
+  <si>
+    <t>can the car be placed in accessories mode?</t>
+  </si>
+  <si>
+    <t>worst case scenario call a mobile mechanic bah</t>
+  </si>
+  <si>
+    <t>In the worst case scenario, you can  probably call a mobile mechanic</t>
+  </si>
+  <si>
+    <t>bah</t>
+  </si>
+  <si>
+    <t>soften command, suggestion</t>
+  </si>
+  <si>
+    <t>I like the watermark  very good very nice</t>
+  </si>
+  <si>
+    <t>I like the watermark; very good, very nice</t>
+  </si>
+  <si>
+    <t>thank you bro new design ah 🤓</t>
+  </si>
+  <si>
+    <t>thank you bro, is this a new design? 🤓</t>
+  </si>
+  <si>
+    <t>I know settled alr   but next time if it happens can check starter motor fuse in the fuse box too   sometimes the fuse blown Haha</t>
+  </si>
+  <si>
+    <t>I know this is already settled but next time if it happens, you can check the starter motor fuse in the fuse box too. Sometimes the fuse has blown</t>
+  </si>
+  <si>
+    <t>just make sure vtec solenoid opens every so often 😛</t>
+  </si>
+  <si>
+    <t>just make sure the vtec solenoid opens every so often 😛</t>
+  </si>
+  <si>
+    <t>the crazy racist mrt lady from hwa chong was there</t>
+  </si>
+  <si>
+    <t>more rare than lbwk avent bro</t>
+  </si>
+  <si>
+    <t>it is more rare than lbwk avent bro</t>
+  </si>
+  <si>
+    <t>@/thoseat mw jn yall can try spot yourselves here</t>
+  </si>
+  <si>
+    <t>wasn't he in this chat once</t>
+  </si>
+  <si>
+    <t>wasn't he in this chat previously?</t>
+  </si>
+  <si>
+    <t>My favourite is squidward from SpongeBob</t>
+  </si>
+  <si>
+    <t>My favourite character is squidward from SpongeBob</t>
+  </si>
+  <si>
+    <t>You know what’s so iconic about this car is that if you say the license plate out loud  it’s “sexy”</t>
+  </si>
+  <si>
+    <t>You know what’s so iconic about this car is that if you say the license plate out loud it’s “sexy”</t>
+  </si>
+  <si>
+    <t>Where is the exact location of this place? So when i come back to sg  i know where I'm gonna spot.Thank you!</t>
+  </si>
+  <si>
+    <t>Where is the exact location of this place? So that when i come back to sg, i know where I'm gonna try to spot it. Thank you!</t>
+  </si>
+  <si>
+    <t>Saw the yellow top taxi again</t>
+  </si>
+  <si>
+    <t>josh are u also a yellow top</t>
+  </si>
+  <si>
+    <t>Join this group to get updates:https://t.me/sgcarmeets</t>
+  </si>
+  <si>
+    <t>bro i nearly banned u on instinct</t>
+  </si>
+  <si>
+    <t>bro, i have nearly banned u out of instinct</t>
+  </si>
+  <si>
+    <t>no la i think is those premium one go airport pickup those ppl one</t>
+  </si>
+  <si>
+    <t>nah i think they are the premium ones that are used to fetch those passengers from the airport</t>
+  </si>
+  <si>
+    <t>Then this one is the other cab company competition</t>
+  </si>
+  <si>
+    <t>Then this is the other competition of the cab company</t>
+  </si>
+  <si>
+    <t>wah nice. hope its gonna come out of the dealership for good soon</t>
+  </si>
+  <si>
+    <t>wow that's nice. hopefully it's gonna come out of the dealership for good soon</t>
+  </si>
+  <si>
+    <t>[Ad Message]Shell has sent SCM information on a special promotion this May and we’d like to share it with you guys!From 3-5 May and 10-12 May  you can fuel up with Shell’s V Power for the price of Shell FuelSave 98!Enjoy maximum engine performance with Shell V-Power which 100% cleans critical engine parts  designed to help your engine run more efficiently and perform at its best. Fill after fill  Drive after drive.More information on Shell V-Power at the promotional price of Shell FuelSave 98 can be foundhere:www.shell.com.sg/shellvpowerV-Power promotion:📍 Any Shell Singapore gas stations📆 3 May  7am to 5 May  10pm</t>
+  </si>
+  <si>
+    <t>[Ad Message]From 2 – 31 May  enjoy manual car washes at only S$8 per wash (U.P S$12) when you fuel up with Shell V-Power! This offer entitles you to UNLIMITED REDEMPTIONS FOR 30 DAYS*!• For existing Shell GO+ members◦ Enjoy a car wash at only S$8 per wash when youaccumulate 60L of Shell V-Power pumped.• For new Shell GO+ members◦ Enjoy a manual car wash for only S$8 withS$88 spent on Shell V-Powerin the same single transaction.Promotion conditions- S$8 per car wash apply to Sedans  MPVs  and SUVs only.- $8 per car wash voucher will be valid for 30 days and up to 99x redemptions*- Shell Car Wash can be found at the following stations:Shell Car Wash | Shell Singapore- Visithttps://shell.com.sg/Vpowerfor more information📍 All Shell Singapore gas stations📆 2-31 May 2024</t>
+  </si>
+  <si>
+    <t>scm members got special discount anot</t>
+  </si>
+  <si>
+    <t>are there any special discounts for scm members</t>
+  </si>
+  <si>
+    <t>i don't think ppl that pump v-power will subject their cars to a shell wash lol</t>
+  </si>
+  <si>
+    <t>i don't think ppl that uses v-power petrol will subject their cars to a car wash at shell lol</t>
+  </si>
+  <si>
+    <t>2025-06-02T11-09-35-953Z</t>
+  </si>
+  <si>
+    <t>inputs/SGTalk_messages270_part3.csv</t>
+  </si>
+  <si>
+    <t>no siaolang is kinda fun to certain extend</t>
+  </si>
+  <si>
+    <t>no crazy people is kinda fun to a certain extend</t>
+  </si>
+  <si>
+    <t>i told her a lame ass joke that i doubt my friends would laugh</t>
+  </si>
+  <si>
+    <t>i told her a lame ass joke that i doubt my friends would even laugh</t>
   </si>
   <si>
     <t>Name</t>
@@ -51839,524 +52130,1352 @@
       </c>
     </row>
     <row r="1615">
-      <c r="A1615" s="1"/>
-      <c r="B1615" s="2"/>
-      <c r="C1615" s="2"/>
-      <c r="D1615" s="2"/>
-      <c r="E1615" s="2"/>
-      <c r="F1615" s="2"/>
-      <c r="G1615" s="2"/>
-      <c r="H1615" s="2"/>
+      <c r="A1615" s="1">
+        <v>45808.44917280093</v>
+      </c>
+      <c r="B1615" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1615" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1615" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1615" s="2" t="s">
+        <v>3006</v>
+      </c>
+      <c r="F1615" s="2" t="s">
+        <v>3007</v>
+      </c>
+      <c r="G1615" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1615" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1616">
-      <c r="A1616" s="1"/>
-      <c r="B1616" s="2"/>
-      <c r="C1616" s="2"/>
-      <c r="D1616" s="2"/>
-      <c r="E1616" s="2"/>
-      <c r="F1616" s="2"/>
-      <c r="G1616" s="2"/>
-      <c r="H1616" s="2"/>
+      <c r="A1616" s="1">
+        <v>45808.45120962963</v>
+      </c>
+      <c r="B1616" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1616" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1616" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1616" s="2" t="s">
+        <v>3008</v>
+      </c>
+      <c r="F1616" s="2" t="s">
+        <v>3009</v>
+      </c>
+      <c r="G1616" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1616" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1617">
-      <c r="A1617" s="1"/>
-      <c r="B1617" s="2"/>
-      <c r="C1617" s="2"/>
-      <c r="D1617" s="2"/>
-      <c r="E1617" s="2"/>
-      <c r="F1617" s="2"/>
-      <c r="G1617" s="2"/>
-      <c r="H1617" s="2"/>
+      <c r="A1617" s="1">
+        <v>45808.45131878472</v>
+      </c>
+      <c r="B1617" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1617" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1617" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1617" s="2" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1617" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1617" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1617" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1618">
-      <c r="A1618" s="1"/>
-      <c r="B1618" s="2"/>
-      <c r="C1618" s="2"/>
-      <c r="D1618" s="2"/>
-      <c r="E1618" s="2"/>
+      <c r="A1618" s="1">
+        <v>45808.451482951394</v>
+      </c>
+      <c r="B1618" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1618" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1618" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1618" s="2" t="s">
+        <v>3011</v>
+      </c>
       <c r="F1618" s="2"/>
-      <c r="G1618" s="2"/>
-      <c r="H1618" s="2"/>
+      <c r="G1618" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1618" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1619">
-      <c r="A1619" s="1"/>
-      <c r="B1619" s="2"/>
-      <c r="C1619" s="2"/>
-      <c r="D1619" s="2"/>
-      <c r="E1619" s="2"/>
-      <c r="F1619" s="2"/>
-      <c r="G1619" s="2"/>
-      <c r="H1619" s="2"/>
+      <c r="A1619" s="1">
+        <v>45808.45176675926</v>
+      </c>
+      <c r="B1619" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1619" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1619" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1619" s="2" t="s">
+        <v>3012</v>
+      </c>
+      <c r="F1619" s="2" t="s">
+        <v>3013</v>
+      </c>
+      <c r="G1619" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1619" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1620">
-      <c r="A1620" s="1"/>
-      <c r="B1620" s="2"/>
-      <c r="C1620" s="2"/>
-      <c r="D1620" s="2"/>
-      <c r="E1620" s="2"/>
-      <c r="F1620" s="2"/>
-      <c r="G1620" s="2"/>
-      <c r="H1620" s="2"/>
+      <c r="A1620" s="1">
+        <v>45808.452427083335</v>
+      </c>
+      <c r="B1620" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1620" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1620" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1620" s="2" t="s">
+        <v>3014</v>
+      </c>
+      <c r="F1620" s="2" t="s">
+        <v>3015</v>
+      </c>
+      <c r="G1620" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1620" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1621">
-      <c r="A1621" s="1"/>
-      <c r="B1621" s="2"/>
-      <c r="C1621" s="2"/>
-      <c r="D1621" s="2"/>
-      <c r="E1621" s="2"/>
-      <c r="F1621" s="2"/>
-      <c r="G1621" s="2"/>
-      <c r="H1621" s="2"/>
+      <c r="A1621" s="1">
+        <v>45808.45310059028</v>
+      </c>
+      <c r="B1621" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1621" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1621" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1621" s="2" t="s">
+        <v>3016</v>
+      </c>
+      <c r="F1621" s="2" t="s">
+        <v>3017</v>
+      </c>
+      <c r="G1621" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1621" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1622">
-      <c r="A1622" s="1"/>
-      <c r="B1622" s="2"/>
-      <c r="C1622" s="2"/>
-      <c r="D1622" s="2"/>
-      <c r="E1622" s="2"/>
-      <c r="F1622" s="2"/>
-      <c r="G1622" s="2"/>
-      <c r="H1622" s="2"/>
+      <c r="A1622" s="1">
+        <v>45808.45356219907</v>
+      </c>
+      <c r="B1622" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1622" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1622" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1622" s="2" t="s">
+        <v>3018</v>
+      </c>
+      <c r="F1622" s="2" t="s">
+        <v>3019</v>
+      </c>
+      <c r="G1622" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1622" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1623">
-      <c r="A1623" s="1"/>
-      <c r="B1623" s="2"/>
-      <c r="C1623" s="2"/>
-      <c r="D1623" s="2"/>
-      <c r="E1623" s="2"/>
-      <c r="F1623" s="2"/>
-      <c r="G1623" s="2"/>
-      <c r="H1623" s="2"/>
+      <c r="A1623" s="1">
+        <v>45808.45405</v>
+      </c>
+      <c r="B1623" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1623" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1623" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1623" s="2" t="s">
+        <v>3020</v>
+      </c>
+      <c r="F1623" s="2" t="s">
+        <v>3021</v>
+      </c>
+      <c r="G1623" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1623" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1624">
-      <c r="A1624" s="1"/>
-      <c r="B1624" s="2"/>
-      <c r="C1624" s="2"/>
-      <c r="D1624" s="2"/>
-      <c r="E1624" s="2"/>
-      <c r="F1624" s="2"/>
-      <c r="G1624" s="2"/>
-      <c r="H1624" s="2"/>
+      <c r="A1624" s="1">
+        <v>45808.454365011574</v>
+      </c>
+      <c r="B1624" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1624" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1624" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1624" s="2" t="s">
+        <v>3022</v>
+      </c>
+      <c r="F1624" s="2" t="s">
+        <v>3023</v>
+      </c>
+      <c r="G1624" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1624" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1625">
-      <c r="A1625" s="1"/>
-      <c r="B1625" s="2"/>
-      <c r="C1625" s="2"/>
-      <c r="D1625" s="2"/>
-      <c r="E1625" s="2"/>
-      <c r="F1625" s="2"/>
-      <c r="G1625" s="2"/>
-      <c r="H1625" s="2"/>
+      <c r="A1625" s="1">
+        <v>45808.45449957176</v>
+      </c>
+      <c r="B1625" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1625" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1625" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1625" s="2" t="s">
+        <v>3024</v>
+      </c>
+      <c r="F1625" s="2" t="s">
+        <v>3025</v>
+      </c>
+      <c r="G1625" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1625" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1626">
-      <c r="A1626" s="1"/>
-      <c r="B1626" s="2"/>
-      <c r="C1626" s="2"/>
-      <c r="D1626" s="2"/>
-      <c r="E1626" s="2"/>
-      <c r="F1626" s="2"/>
-      <c r="G1626" s="2"/>
-      <c r="H1626" s="2"/>
+      <c r="A1626" s="1">
+        <v>45808.45493457176</v>
+      </c>
+      <c r="B1626" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1626" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1626" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1626" s="2" t="s">
+        <v>3026</v>
+      </c>
+      <c r="F1626" s="2" t="s">
+        <v>3027</v>
+      </c>
+      <c r="G1626" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1626" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1627">
-      <c r="A1627" s="1"/>
-      <c r="B1627" s="2"/>
-      <c r="C1627" s="2"/>
-      <c r="D1627" s="2"/>
-      <c r="E1627" s="2"/>
-      <c r="F1627" s="2"/>
-      <c r="G1627" s="2"/>
-      <c r="H1627" s="2"/>
+      <c r="A1627" s="1">
+        <v>45808.45520096065</v>
+      </c>
+      <c r="B1627" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1627" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1627" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1627" s="2" t="s">
+        <v>3028</v>
+      </c>
+      <c r="F1627" s="2" t="s">
+        <v>3029</v>
+      </c>
+      <c r="G1627" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1627" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1628">
-      <c r="A1628" s="1"/>
-      <c r="B1628" s="2"/>
-      <c r="C1628" s="2"/>
-      <c r="D1628" s="2"/>
-      <c r="E1628" s="2"/>
-      <c r="F1628" s="2"/>
-      <c r="G1628" s="2"/>
-      <c r="H1628" s="2"/>
+      <c r="A1628" s="1">
+        <v>45808.455328634256</v>
+      </c>
+      <c r="B1628" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1628" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1628" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1628" s="2" t="s">
+        <v>3030</v>
+      </c>
+      <c r="F1628" s="2" t="s">
+        <v>3031</v>
+      </c>
+      <c r="G1628" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1628" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1629">
-      <c r="A1629" s="1"/>
-      <c r="B1629" s="2"/>
-      <c r="C1629" s="2"/>
-      <c r="D1629" s="2"/>
-      <c r="E1629" s="2"/>
-      <c r="F1629" s="2"/>
-      <c r="G1629" s="2"/>
-      <c r="H1629" s="2"/>
+      <c r="A1629" s="1">
+        <v>45808.45546935185</v>
+      </c>
+      <c r="B1629" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1629" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1629" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1629" s="2" t="s">
+        <v>3032</v>
+      </c>
+      <c r="F1629" s="2" t="s">
+        <v>3033</v>
+      </c>
+      <c r="G1629" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1629" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1630">
-      <c r="A1630" s="1"/>
-      <c r="B1630" s="2"/>
-      <c r="C1630" s="2"/>
-      <c r="D1630" s="2"/>
-      <c r="E1630" s="2"/>
-      <c r="F1630" s="2"/>
-      <c r="G1630" s="2"/>
-      <c r="H1630" s="2"/>
+      <c r="A1630" s="1">
+        <v>45808.45561534722</v>
+      </c>
+      <c r="B1630" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1630" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1630" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1630" s="2" t="s">
+        <v>3034</v>
+      </c>
+      <c r="F1630" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1630" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1630" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1631">
-      <c r="A1631" s="1"/>
-      <c r="B1631" s="2"/>
-      <c r="C1631" s="2"/>
-      <c r="D1631" s="2"/>
-      <c r="E1631" s="2"/>
-      <c r="F1631" s="2"/>
-      <c r="G1631" s="2"/>
-      <c r="H1631" s="2"/>
+      <c r="A1631" s="1">
+        <v>45808.455799664356</v>
+      </c>
+      <c r="B1631" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1631" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1631" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1631" s="2" t="s">
+        <v>3035</v>
+      </c>
+      <c r="F1631" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1631" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1631" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1632">
-      <c r="A1632" s="1"/>
-      <c r="B1632" s="2"/>
-      <c r="C1632" s="2"/>
-      <c r="D1632" s="2"/>
-      <c r="E1632" s="2"/>
-      <c r="F1632" s="2"/>
-      <c r="G1632" s="2"/>
-      <c r="H1632" s="2"/>
+      <c r="A1632" s="1">
+        <v>45808.45601596065</v>
+      </c>
+      <c r="B1632" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1632" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1632" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1632" s="2" t="s">
+        <v>3036</v>
+      </c>
+      <c r="F1632" s="2" t="s">
+        <v>3037</v>
+      </c>
+      <c r="G1632" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1632" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1633">
-      <c r="A1633" s="1"/>
-      <c r="B1633" s="2"/>
-      <c r="C1633" s="2"/>
-      <c r="D1633" s="2"/>
-      <c r="E1633" s="2"/>
-      <c r="F1633" s="2"/>
-      <c r="G1633" s="2"/>
-      <c r="H1633" s="2"/>
+      <c r="A1633" s="1">
+        <v>45808.45616563657</v>
+      </c>
+      <c r="B1633" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1633" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1633" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1633" s="2" t="s">
+        <v>3038</v>
+      </c>
+      <c r="F1633" s="2" t="s">
+        <v>3039</v>
+      </c>
+      <c r="G1633" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1633" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1634">
-      <c r="A1634" s="1"/>
-      <c r="B1634" s="2"/>
-      <c r="C1634" s="2"/>
-      <c r="D1634" s="2"/>
-      <c r="E1634" s="2"/>
-      <c r="F1634" s="2"/>
-      <c r="G1634" s="2"/>
-      <c r="H1634" s="2"/>
+      <c r="A1634" s="1">
+        <v>45808.45639921296</v>
+      </c>
+      <c r="B1634" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1634" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1634" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1634" s="2" t="s">
+        <v>3040</v>
+      </c>
+      <c r="F1634" s="2" t="s">
+        <v>3041</v>
+      </c>
+      <c r="G1634" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1634" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1635">
-      <c r="A1635" s="1"/>
-      <c r="B1635" s="2"/>
-      <c r="C1635" s="2"/>
-      <c r="D1635" s="2"/>
-      <c r="E1635" s="2"/>
-      <c r="F1635" s="2"/>
-      <c r="G1635" s="2"/>
-      <c r="H1635" s="2"/>
+      <c r="A1635" s="1">
+        <v>45808.45657717592</v>
+      </c>
+      <c r="B1635" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1635" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1635" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1635" s="2" t="s">
+        <v>3042</v>
+      </c>
+      <c r="F1635" s="2" t="s">
+        <v>3042</v>
+      </c>
+      <c r="G1635" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1635" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1636">
-      <c r="A1636" s="1"/>
-      <c r="B1636" s="2"/>
-      <c r="C1636" s="2"/>
-      <c r="D1636" s="2"/>
-      <c r="E1636" s="2"/>
-      <c r="F1636" s="2"/>
-      <c r="G1636" s="2"/>
-      <c r="H1636" s="2"/>
+      <c r="A1636" s="1">
+        <v>45808.45676457176</v>
+      </c>
+      <c r="B1636" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1636" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1636" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1636" s="2" t="s">
+        <v>3043</v>
+      </c>
+      <c r="F1636" s="2" t="s">
+        <v>3044</v>
+      </c>
+      <c r="G1636" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1636" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1637">
-      <c r="A1637" s="1"/>
-      <c r="B1637" s="2"/>
-      <c r="C1637" s="2"/>
-      <c r="D1637" s="2"/>
-      <c r="E1637" s="2"/>
-      <c r="F1637" s="2"/>
-      <c r="G1637" s="2"/>
-      <c r="H1637" s="2"/>
+      <c r="A1637" s="1">
+        <v>45808.45707229167</v>
+      </c>
+      <c r="B1637" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1637" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1637" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1637" s="2" t="s">
+        <v>3045</v>
+      </c>
+      <c r="F1637" s="2" t="s">
+        <v>3046</v>
+      </c>
+      <c r="G1637" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1637" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1637" s="2" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="1638">
-      <c r="A1638" s="1"/>
-      <c r="B1638" s="2"/>
-      <c r="C1638" s="2"/>
-      <c r="D1638" s="2"/>
-      <c r="E1638" s="2"/>
-      <c r="F1638" s="2"/>
-      <c r="G1638" s="2"/>
-      <c r="H1638" s="2"/>
+      <c r="A1638" s="1">
+        <v>45808.45726768518</v>
+      </c>
+      <c r="B1638" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1638" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1638" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1638" s="2" t="s">
+        <v>3047</v>
+      </c>
+      <c r="F1638" s="2" t="s">
+        <v>3048</v>
+      </c>
+      <c r="G1638" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1638" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1639">
-      <c r="A1639" s="1"/>
-      <c r="B1639" s="2"/>
-      <c r="C1639" s="2"/>
-      <c r="D1639" s="2"/>
-      <c r="E1639" s="2"/>
-      <c r="F1639" s="2"/>
-      <c r="G1639" s="2"/>
-      <c r="H1639" s="2"/>
+      <c r="A1639" s="1">
+        <v>45808.45741505787</v>
+      </c>
+      <c r="B1639" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1639" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1639" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1639" s="2" t="s">
+        <v>3049</v>
+      </c>
+      <c r="F1639" s="2" t="s">
+        <v>3050</v>
+      </c>
+      <c r="G1639" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1639" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1640">
-      <c r="A1640" s="1"/>
-      <c r="B1640" s="2"/>
-      <c r="C1640" s="2"/>
-      <c r="D1640" s="2"/>
-      <c r="E1640" s="2"/>
-      <c r="F1640" s="2"/>
-      <c r="G1640" s="2"/>
-      <c r="H1640" s="2"/>
+      <c r="A1640" s="1">
+        <v>45808.45756082176</v>
+      </c>
+      <c r="B1640" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1640" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1640" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1640" s="2" t="s">
+        <v>3051</v>
+      </c>
+      <c r="F1640" s="2" t="s">
+        <v>3052</v>
+      </c>
+      <c r="G1640" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1640" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1641">
-      <c r="A1641" s="1"/>
-      <c r="B1641" s="2"/>
-      <c r="C1641" s="2"/>
-      <c r="D1641" s="2"/>
-      <c r="E1641" s="2"/>
-      <c r="F1641" s="2"/>
-      <c r="G1641" s="2"/>
-      <c r="H1641" s="2"/>
+      <c r="A1641" s="1">
+        <v>45808.457657858795</v>
+      </c>
+      <c r="B1641" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1641" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1641" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1641" s="2" t="s">
+        <v>3053</v>
+      </c>
+      <c r="F1641" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1641" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1641" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1642">
-      <c r="A1642" s="1"/>
-      <c r="B1642" s="2"/>
-      <c r="C1642" s="2"/>
-      <c r="D1642" s="2"/>
-      <c r="E1642" s="2"/>
-      <c r="F1642" s="2"/>
-      <c r="G1642" s="2"/>
-      <c r="H1642" s="2"/>
+      <c r="A1642" s="1">
+        <v>45808.458154733795</v>
+      </c>
+      <c r="B1642" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1642" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1642" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1642" s="2" t="s">
+        <v>3054</v>
+      </c>
+      <c r="F1642" s="2" t="s">
+        <v>3055</v>
+      </c>
+      <c r="G1642" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1642" s="2" t="s">
+        <v>3056</v>
+      </c>
+      <c r="I1642" s="2" t="s">
+        <v>3057</v>
+      </c>
     </row>
     <row r="1643">
-      <c r="A1643" s="1"/>
-      <c r="B1643" s="2"/>
-      <c r="C1643" s="2"/>
-      <c r="D1643" s="2"/>
-      <c r="E1643" s="2"/>
-      <c r="F1643" s="2"/>
-      <c r="G1643" s="2"/>
-      <c r="H1643" s="2"/>
+      <c r="A1643" s="1">
+        <v>45808.458302037034</v>
+      </c>
+      <c r="B1643" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1643" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1643" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1643" s="2" t="s">
+        <v>3058</v>
+      </c>
+      <c r="F1643" s="2" t="s">
+        <v>3059</v>
+      </c>
+      <c r="G1643" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1643" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1644">
-      <c r="A1644" s="1"/>
-      <c r="B1644" s="2"/>
-      <c r="C1644" s="2"/>
-      <c r="D1644" s="2"/>
-      <c r="E1644" s="2"/>
-      <c r="F1644" s="2"/>
-      <c r="G1644" s="2"/>
-      <c r="H1644" s="2"/>
+      <c r="A1644" s="1">
+        <v>45808.45844545139</v>
+      </c>
+      <c r="B1644" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1644" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1644" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1644" s="2" t="s">
+        <v>3060</v>
+      </c>
+      <c r="F1644" s="2" t="s">
+        <v>3061</v>
+      </c>
+      <c r="G1644" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1644" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1645">
-      <c r="A1645" s="1"/>
-      <c r="B1645" s="2"/>
-      <c r="C1645" s="2"/>
-      <c r="D1645" s="2"/>
-      <c r="E1645" s="2"/>
-      <c r="F1645" s="2"/>
-      <c r="G1645" s="2"/>
-      <c r="H1645" s="2"/>
+      <c r="A1645" s="1">
+        <v>45808.45878752315</v>
+      </c>
+      <c r="B1645" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1645" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1645" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1645" s="2" t="s">
+        <v>3062</v>
+      </c>
+      <c r="F1645" s="2" t="s">
+        <v>3063</v>
+      </c>
+      <c r="G1645" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1645" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1646">
-      <c r="A1646" s="1"/>
-      <c r="B1646" s="2"/>
-      <c r="C1646" s="2"/>
-      <c r="D1646" s="2"/>
-      <c r="E1646" s="2"/>
-      <c r="F1646" s="2"/>
-      <c r="G1646" s="2"/>
-      <c r="H1646" s="2"/>
+      <c r="A1646" s="1">
+        <v>45808.45912587963</v>
+      </c>
+      <c r="B1646" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1646" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1646" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1646" s="2" t="s">
+        <v>3064</v>
+      </c>
+      <c r="F1646" s="2" t="s">
+        <v>3065</v>
+      </c>
+      <c r="G1646" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1646" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1647">
-      <c r="A1647" s="1"/>
-      <c r="B1647" s="2"/>
-      <c r="C1647" s="2"/>
-      <c r="D1647" s="2"/>
-      <c r="E1647" s="2"/>
-      <c r="F1647" s="2"/>
-      <c r="G1647" s="2"/>
-      <c r="H1647" s="2"/>
+      <c r="A1647" s="1">
+        <v>45808.459303298616</v>
+      </c>
+      <c r="B1647" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1647" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1647" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1647" s="2" t="s">
+        <v>3066</v>
+      </c>
+      <c r="F1647" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1647" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1647" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1648">
-      <c r="A1648" s="1"/>
-      <c r="B1648" s="2"/>
-      <c r="C1648" s="2"/>
-      <c r="D1648" s="2"/>
-      <c r="E1648" s="2"/>
-      <c r="F1648" s="2"/>
-      <c r="G1648" s="2"/>
-      <c r="H1648" s="2"/>
+      <c r="A1648" s="1">
+        <v>45808.459435613426</v>
+      </c>
+      <c r="B1648" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1648" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1648" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1648" s="2" t="s">
+        <v>3067</v>
+      </c>
+      <c r="F1648" s="2" t="s">
+        <v>3068</v>
+      </c>
+      <c r="G1648" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1648" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1649">
-      <c r="A1649" s="1"/>
-      <c r="B1649" s="2"/>
-      <c r="C1649" s="2"/>
-      <c r="D1649" s="2"/>
-      <c r="E1649" s="2"/>
+      <c r="A1649" s="1">
+        <v>45808.45960565972</v>
+      </c>
+      <c r="B1649" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1649" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1649" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1649" s="2" t="s">
+        <v>3069</v>
+      </c>
       <c r="F1649" s="2"/>
-      <c r="G1649" s="2"/>
-      <c r="H1649" s="2"/>
+      <c r="G1649" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1649" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1650">
-      <c r="A1650" s="1"/>
-      <c r="B1650" s="2"/>
-      <c r="C1650" s="2"/>
-      <c r="D1650" s="2"/>
-      <c r="E1650" s="2"/>
-      <c r="F1650" s="2"/>
-      <c r="G1650" s="2"/>
-      <c r="H1650" s="2"/>
+      <c r="A1650" s="1">
+        <v>45808.45971542824</v>
+      </c>
+      <c r="B1650" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1650" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1650" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1650" s="2" t="s">
+        <v>3070</v>
+      </c>
+      <c r="F1650" s="2" t="s">
+        <v>3071</v>
+      </c>
+      <c r="G1650" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1650" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1651">
-      <c r="A1651" s="1"/>
-      <c r="B1651" s="2"/>
-      <c r="C1651" s="2"/>
-      <c r="D1651" s="2"/>
-      <c r="E1651" s="2"/>
-      <c r="F1651" s="2"/>
-      <c r="G1651" s="2"/>
-      <c r="H1651" s="2"/>
+      <c r="A1651" s="1">
+        <v>45808.45983600694</v>
+      </c>
+      <c r="B1651" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1651" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1651" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1651" s="2" t="s">
+        <v>3072</v>
+      </c>
+      <c r="F1651" s="2" t="s">
+        <v>3073</v>
+      </c>
+      <c r="G1651" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1651" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1652">
-      <c r="A1652" s="1"/>
-      <c r="B1652" s="2"/>
-      <c r="C1652" s="2"/>
-      <c r="D1652" s="2"/>
-      <c r="E1652" s="2"/>
-      <c r="F1652" s="2"/>
-      <c r="G1652" s="2"/>
-      <c r="H1652" s="2"/>
+      <c r="A1652" s="1">
+        <v>45808.4600619213</v>
+      </c>
+      <c r="B1652" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1652" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1652" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1652" s="2" t="s">
+        <v>3074</v>
+      </c>
+      <c r="F1652" s="2" t="s">
+        <v>3075</v>
+      </c>
+      <c r="G1652" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1652" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1653">
-      <c r="A1653" s="1"/>
-      <c r="B1653" s="2"/>
-      <c r="C1653" s="2"/>
-      <c r="D1653" s="2"/>
-      <c r="E1653" s="2"/>
-      <c r="F1653" s="2"/>
-      <c r="G1653" s="2"/>
-      <c r="H1653" s="2"/>
+      <c r="A1653" s="1">
+        <v>45808.46040546296</v>
+      </c>
+      <c r="B1653" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1653" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1653" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1653" s="2" t="s">
+        <v>3076</v>
+      </c>
+      <c r="F1653" s="2" t="s">
+        <v>3077</v>
+      </c>
+      <c r="G1653" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1653" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1654">
-      <c r="A1654" s="1"/>
-      <c r="B1654" s="2"/>
-      <c r="C1654" s="2"/>
-      <c r="D1654" s="2"/>
-      <c r="E1654" s="2"/>
-      <c r="F1654" s="2"/>
-      <c r="G1654" s="2"/>
-      <c r="H1654" s="2"/>
+      <c r="A1654" s="1">
+        <v>45808.46049790509</v>
+      </c>
+      <c r="B1654" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1654" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1654" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1654" s="2" t="s">
+        <v>3078</v>
+      </c>
+      <c r="F1654" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1654" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1654" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1655">
-      <c r="A1655" s="1"/>
-      <c r="B1655" s="2"/>
-      <c r="C1655" s="2"/>
-      <c r="D1655" s="2"/>
-      <c r="E1655" s="2"/>
-      <c r="F1655" s="2"/>
-      <c r="G1655" s="2"/>
-      <c r="H1655" s="2"/>
+      <c r="A1655" s="1">
+        <v>45808.46056767361</v>
+      </c>
+      <c r="B1655" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1655" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1655" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1655" s="2" t="s">
+        <v>3079</v>
+      </c>
+      <c r="F1655" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1655" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1655" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1656">
-      <c r="A1656" s="1"/>
-      <c r="B1656" s="2"/>
-      <c r="C1656" s="2"/>
-      <c r="D1656" s="2"/>
-      <c r="E1656" s="2"/>
+      <c r="A1656" s="1">
+        <v>45808.460605115746</v>
+      </c>
+      <c r="B1656" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1656" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1656" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1656" s="2" t="s">
+        <v>3080</v>
+      </c>
       <c r="F1656" s="2"/>
-      <c r="G1656" s="2"/>
-      <c r="H1656" s="2"/>
+      <c r="G1656" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1656" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1657">
-      <c r="A1657" s="1"/>
-      <c r="B1657" s="2"/>
-      <c r="C1657" s="2"/>
-      <c r="D1657" s="2"/>
-      <c r="E1657" s="2"/>
-      <c r="F1657" s="2"/>
-      <c r="G1657" s="2"/>
-      <c r="H1657" s="2"/>
+      <c r="A1657" s="1">
+        <v>45808.46082854166</v>
+      </c>
+      <c r="B1657" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1657" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1657" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1657" s="2" t="s">
+        <v>3081</v>
+      </c>
+      <c r="F1657" s="2" t="s">
+        <v>3082</v>
+      </c>
+      <c r="G1657" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1657" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1658">
-      <c r="A1658" s="1"/>
-      <c r="B1658" s="2"/>
-      <c r="C1658" s="2"/>
-      <c r="D1658" s="2"/>
-      <c r="E1658" s="2"/>
-      <c r="F1658" s="2"/>
-      <c r="G1658" s="2"/>
-      <c r="H1658" s="2"/>
+      <c r="A1658" s="1">
+        <v>45808.461621863426</v>
+      </c>
+      <c r="B1658" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1658" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1658" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1658" s="2" t="s">
+        <v>3083</v>
+      </c>
+      <c r="F1658" s="2" t="s">
+        <v>3084</v>
+      </c>
+      <c r="G1658" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1658" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1659">
-      <c r="A1659" s="1"/>
-      <c r="B1659" s="2"/>
-      <c r="C1659" s="2"/>
-      <c r="D1659" s="2"/>
-      <c r="E1659" s="2"/>
-      <c r="F1659" s="2"/>
-      <c r="G1659" s="2"/>
-      <c r="H1659" s="2"/>
+      <c r="A1659" s="1">
+        <v>45810.29663891204</v>
+      </c>
+      <c r="B1659" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1659" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1659" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1659" s="2" t="s">
+        <v>3085</v>
+      </c>
+      <c r="F1659" s="2" t="s">
+        <v>3086</v>
+      </c>
+      <c r="G1659" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1659" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1660">
-      <c r="A1660" s="1"/>
-      <c r="B1660" s="2"/>
-      <c r="C1660" s="2"/>
-      <c r="D1660" s="2"/>
-      <c r="E1660" s="2"/>
-      <c r="F1660" s="2"/>
-      <c r="G1660" s="2"/>
-      <c r="H1660" s="2"/>
+      <c r="A1660" s="1">
+        <v>45810.29686731481</v>
+      </c>
+      <c r="B1660" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1660" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1660" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1660" s="2" t="s">
+        <v>3087</v>
+      </c>
+      <c r="F1660" s="2" t="s">
+        <v>3088</v>
+      </c>
+      <c r="G1660" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1660" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1661">
-      <c r="A1661" s="1"/>
-      <c r="B1661" s="2"/>
-      <c r="C1661" s="2"/>
-      <c r="D1661" s="2"/>
-      <c r="E1661" s="2"/>
+      <c r="A1661" s="1">
+        <v>45810.29693453704</v>
+      </c>
+      <c r="B1661" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1661" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1661" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1661" s="2" t="s">
+        <v>3089</v>
+      </c>
       <c r="F1661" s="2"/>
-      <c r="G1661" s="2"/>
-      <c r="H1661" s="2"/>
+      <c r="G1661" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1661" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1662">
-      <c r="A1662" s="1"/>
-      <c r="B1662" s="2"/>
-      <c r="C1662" s="2"/>
-      <c r="D1662" s="2"/>
-      <c r="E1662" s="2"/>
+      <c r="A1662" s="1">
+        <v>45810.29697386574</v>
+      </c>
+      <c r="B1662" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1662" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1662" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1662" s="2" t="s">
+        <v>3090</v>
+      </c>
       <c r="F1662" s="2"/>
-      <c r="G1662" s="2"/>
-      <c r="H1662" s="2"/>
+      <c r="G1662" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1662" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1663">
-      <c r="A1663" s="1"/>
-      <c r="B1663" s="2"/>
-      <c r="C1663" s="2"/>
-      <c r="D1663" s="2"/>
-      <c r="E1663" s="2"/>
-      <c r="F1663" s="2"/>
-      <c r="G1663" s="2"/>
-      <c r="H1663" s="2"/>
+      <c r="A1663" s="1">
+        <v>45810.297208715274</v>
+      </c>
+      <c r="B1663" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1663" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1663" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1663" s="2" t="s">
+        <v>3091</v>
+      </c>
+      <c r="F1663" s="2" t="s">
+        <v>3092</v>
+      </c>
+      <c r="G1663" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1663" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1664">
-      <c r="A1664" s="1"/>
-      <c r="B1664" s="2"/>
-      <c r="C1664" s="2"/>
-      <c r="D1664" s="2"/>
-      <c r="E1664" s="2"/>
-      <c r="F1664" s="2"/>
-      <c r="G1664" s="2"/>
-      <c r="H1664" s="2"/>
+      <c r="A1664" s="1">
+        <v>45810.29768766204</v>
+      </c>
+      <c r="B1664" s="2" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1664" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1664" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="E1664" s="2" t="s">
+        <v>3093</v>
+      </c>
+      <c r="F1664" s="2" t="s">
+        <v>3094</v>
+      </c>
+      <c r="G1664" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1664" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1665">
-      <c r="A1665" s="1"/>
-      <c r="B1665" s="2"/>
-      <c r="C1665" s="2"/>
-      <c r="D1665" s="2"/>
-      <c r="E1665" s="2"/>
-      <c r="F1665" s="2"/>
-      <c r="G1665" s="2"/>
-      <c r="H1665" s="2"/>
+      <c r="A1665" s="1">
+        <v>45810.29850709491</v>
+      </c>
+      <c r="B1665" s="2" t="s">
+        <v>3095</v>
+      </c>
+      <c r="C1665" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1665" s="2" t="s">
+        <v>3096</v>
+      </c>
+      <c r="E1665" s="2" t="s">
+        <v>3097</v>
+      </c>
+      <c r="F1665" s="2" t="s">
+        <v>3098</v>
+      </c>
+      <c r="G1665" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1665" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1666">
-      <c r="A1666" s="1"/>
-      <c r="B1666" s="2"/>
-      <c r="C1666" s="2"/>
-      <c r="D1666" s="2"/>
-      <c r="E1666" s="2"/>
-      <c r="F1666" s="2"/>
-      <c r="G1666" s="2"/>
-      <c r="H1666" s="2"/>
+      <c r="A1666" s="1">
+        <v>45810.29867019676</v>
+      </c>
+      <c r="B1666" s="2" t="s">
+        <v>3095</v>
+      </c>
+      <c r="C1666" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1666" s="2" t="s">
+        <v>3096</v>
+      </c>
+      <c r="E1666" s="2" t="s">
+        <v>3099</v>
+      </c>
+      <c r="F1666" s="2" t="s">
+        <v>3100</v>
+      </c>
+      <c r="G1666" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1666" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="1667">
       <c r="A1667" s="1"/>
@@ -55721,16 +56840,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>3004</v>
+        <v>3101</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>3005</v>
+        <v>3102</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>3006</v>
+        <v>3103</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>3007</v>
+        <v>3104</v>
       </c>
       <c r="F1" s="2">
         <v>1355076.0</v>
@@ -55747,10 +56866,10 @@
       </c>
       <c r="C2" s="5">
         <f t="shared" ref="C2:C7" si="1">NOW()</f>
-        <v>45806.35979</v>
+        <v>45813.31729</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>3008</v>
+        <v>3105</v>
       </c>
       <c r="F2" s="6">
         <f>0.1*F1</f>
@@ -55768,14 +56887,14 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" si="1"/>
-        <v>45806.35979</v>
+        <v>45813.31729</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>3009</v>
+        <v>3106</v>
       </c>
       <c r="F3" s="7">
         <f>SUM(B2:B7)</f>
-        <v>2038</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="4">
@@ -55789,7 +56908,7 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>45806.35979</v>
+        <v>45813.31729</v>
       </c>
     </row>
     <row r="5">
@@ -55803,7 +56922,7 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>45806.35979</v>
+        <v>45813.31729</v>
       </c>
     </row>
     <row r="6">
@@ -55813,11 +56932,11 @@
       </c>
       <c r="B6" s="4">
         <f>COUNTIFS(ALL_TRANSLATIONS!C:C,A6,ALL_TRANSLATIONS!G:G,"&lt;&gt;skipped")</f>
-        <v>439</v>
+        <v>486</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>45806.35979</v>
+        <v>45813.31729</v>
       </c>
     </row>
     <row r="7">
@@ -55827,11 +56946,11 @@
       </c>
       <c r="B7" s="4">
         <f>COUNTIFS(ALL_TRANSLATIONS!C:C,A7,ALL_TRANSLATIONS!G:G,"&lt;&gt;skipped")</f>
-        <v>439</v>
+        <v>486</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>45806.35979</v>
+        <v>45813.31729</v>
       </c>
     </row>
     <row r="8">
@@ -55859,13 +56978,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="8" t="s">
-        <v>3010</v>
+        <v>3107</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3011</v>
+        <v>3108</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3012</v>
+        <v>3109</v>
       </c>
     </row>
     <row r="2">
@@ -55873,7 +56992,7 @@
         <v>2110</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2111</v>
@@ -55884,7 +57003,7 @@
         <v>2112</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2113</v>
@@ -55895,7 +57014,7 @@
         <v>2114</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2115</v>
@@ -55906,7 +57025,7 @@
         <v>2116</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>2117</v>
@@ -55917,7 +57036,7 @@
         <v>2118</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2119</v>
@@ -55928,7 +57047,7 @@
         <v>2120</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>2121</v>
@@ -55939,7 +57058,7 @@
         <v>2122</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>2123</v>
@@ -55950,7 +57069,7 @@
         <v>2124</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>2125</v>
@@ -55961,7 +57080,7 @@
         <v>2126</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2127</v>
@@ -55972,7 +57091,7 @@
         <v>2128</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>2129</v>
@@ -55983,7 +57102,7 @@
         <v>2131</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>2132</v>
@@ -55994,7 +57113,7 @@
         <v>2133</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>2134</v>
@@ -56005,7 +57124,7 @@
         <v>2135</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>2136</v>
@@ -56016,7 +57135,7 @@
         <v>2137</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>2138</v>
@@ -56027,7 +57146,7 @@
         <v>2140</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>2141</v>
@@ -56038,7 +57157,7 @@
         <v>2142</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>2143</v>
@@ -56049,7 +57168,7 @@
         <v>2144</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>2145</v>
@@ -56060,7 +57179,7 @@
         <v>2146</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>2147</v>
@@ -56071,7 +57190,7 @@
         <v>2148</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>2149</v>
@@ -56082,7 +57201,7 @@
         <v>2150</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>2151</v>
@@ -56093,7 +57212,7 @@
         <v>2152</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>2153</v>
@@ -56104,7 +57223,7 @@
         <v>2154</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>2155</v>
@@ -56115,7 +57234,7 @@
         <v>2156</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>2157</v>
@@ -56126,7 +57245,7 @@
         <v>2158</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>2159</v>
@@ -56137,7 +57256,7 @@
         <v>2160</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>2161</v>
@@ -56148,7 +57267,7 @@
         <v>2162</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>2163</v>
@@ -56159,7 +57278,7 @@
         <v>2164</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>2165</v>
@@ -56170,7 +57289,7 @@
         <v>2166</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>2167</v>
@@ -56181,7 +57300,7 @@
         <v>2168</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>2169</v>
@@ -56192,7 +57311,7 @@
         <v>2170</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>2171</v>
@@ -56203,7 +57322,7 @@
         <v>2172</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>2173</v>
@@ -56214,7 +57333,7 @@
         <v>2174</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>2175</v>
@@ -56225,7 +57344,7 @@
         <v>2176</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>2177</v>
@@ -56236,7 +57355,7 @@
         <v>2178</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>2179</v>
@@ -56247,7 +57366,7 @@
         <v>2180</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>2181</v>
@@ -56258,7 +57377,7 @@
         <v>2182</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>2183</v>
@@ -56269,7 +57388,7 @@
         <v>2184</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>2185</v>
@@ -56280,7 +57399,7 @@
         <v>2186</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>2187</v>
@@ -56291,7 +57410,7 @@
         <v>2188</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>2189</v>
@@ -56302,7 +57421,7 @@
         <v>2190</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>2191</v>
@@ -56313,7 +57432,7 @@
         <v>2192</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>2193</v>
@@ -56324,7 +57443,7 @@
         <v>2194</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>2195</v>
@@ -56335,7 +57454,7 @@
         <v>2196</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>2197</v>
@@ -56346,7 +57465,7 @@
         <v>2198</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>2199</v>
@@ -56357,7 +57476,7 @@
         <v>2200</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>2201</v>
@@ -56368,7 +57487,7 @@
         <v>2202</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>2203</v>
@@ -56379,7 +57498,7 @@
         <v>2204</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>2205</v>
@@ -56390,7 +57509,7 @@
         <v>2206</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>2207</v>
@@ -56401,7 +57520,7 @@
         <v>2208</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>2209</v>
@@ -56412,7 +57531,7 @@
         <v>2210</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>2211</v>
@@ -56423,7 +57542,7 @@
         <v>2212</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>2213</v>
@@ -56434,7 +57553,7 @@
         <v>2214</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>2215</v>
@@ -56445,7 +57564,7 @@
         <v>2216</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>2217</v>
@@ -56456,7 +57575,7 @@
         <v>2218</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>2219</v>
@@ -56467,7 +57586,7 @@
         <v>2220</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>2221</v>
@@ -56478,7 +57597,7 @@
         <v>2223</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>2224</v>
@@ -56489,7 +57608,7 @@
         <v>2225</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>2226</v>
@@ -56500,7 +57619,7 @@
         <v>2227</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>2228</v>
@@ -56511,7 +57630,7 @@
         <v>2229</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>2230</v>
@@ -56522,7 +57641,7 @@
         <v>2231</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>2232</v>
@@ -56533,7 +57652,7 @@
         <v>2233</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>2234</v>
@@ -56544,7 +57663,7 @@
         <v>2235</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>2236</v>
@@ -56555,7 +57674,7 @@
         <v>2237</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>2238</v>
@@ -56566,7 +57685,7 @@
         <v>2239</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>2240</v>
@@ -56577,7 +57696,7 @@
         <v>2241</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>2242</v>
@@ -56588,7 +57707,7 @@
         <v>2243</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>2244</v>
@@ -56599,7 +57718,7 @@
         <v>2247</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>2248</v>
@@ -56610,7 +57729,7 @@
         <v>2249</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>2250</v>
@@ -56621,7 +57740,7 @@
         <v>2251</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>2252</v>
@@ -56632,7 +57751,7 @@
         <v>2253</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>72</v>
@@ -56643,7 +57762,7 @@
         <v>2254</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>2255</v>
@@ -56654,7 +57773,7 @@
         <v>2256</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>2257</v>
@@ -56665,7 +57784,7 @@
         <v>2259</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>2260</v>
@@ -56676,7 +57795,7 @@
         <v>2261</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>2262</v>
@@ -56687,7 +57806,7 @@
         <v>2263</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>72</v>
@@ -56698,7 +57817,7 @@
         <v>2264</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>2265</v>
@@ -56709,7 +57828,7 @@
         <v>2266</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>2267</v>
@@ -56720,7 +57839,7 @@
         <v>2268</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>2269</v>
@@ -56731,7 +57850,7 @@
         <v>2270</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>2271</v>
@@ -56742,7 +57861,7 @@
         <v>2272</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>2273</v>
@@ -56753,7 +57872,7 @@
         <v>2275</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>2276</v>
@@ -56764,7 +57883,7 @@
         <v>2278</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>2279</v>
@@ -56775,7 +57894,7 @@
         <v>2280</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>2281</v>
@@ -56786,7 +57905,7 @@
         <v>2282</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>2283</v>
@@ -56797,7 +57916,7 @@
         <v>2284</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>2285</v>
@@ -56808,7 +57927,7 @@
         <v>2286</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>2287</v>
@@ -56819,7 +57938,7 @@
         <v>2288</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>2289</v>
@@ -56830,7 +57949,7 @@
         <v>2291</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>72</v>
@@ -56841,7 +57960,7 @@
         <v>2292</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>2293</v>
@@ -56852,7 +57971,7 @@
         <v>2294</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>2295</v>
@@ -56863,7 +57982,7 @@
         <v>2296</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>2297</v>
@@ -56874,7 +57993,7 @@
         <v>2299</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>2300</v>
@@ -56885,7 +58004,7 @@
         <v>2301</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>72</v>
@@ -56896,7 +58015,7 @@
         <v>2302</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>2303</v>
@@ -56907,7 +58026,7 @@
         <v>2306</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>72</v>
@@ -56918,7 +58037,7 @@
         <v>2307</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>2308</v>
@@ -56929,7 +58048,7 @@
         <v>2309</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>2310</v>
@@ -56940,7 +58059,7 @@
         <v>2311</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>2312</v>
@@ -56951,7 +58070,7 @@
         <v>2313</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>2314</v>
@@ -56962,7 +58081,7 @@
         <v>2315</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>2316</v>
@@ -56973,7 +58092,7 @@
         <v>144</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>145</v>
@@ -56984,7 +58103,7 @@
         <v>146</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>147</v>
@@ -56995,7 +58114,7 @@
         <v>148</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>149</v>
@@ -57006,7 +58125,7 @@
         <v>150</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>151</v>
@@ -57017,7 +58136,7 @@
         <v>154</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>72</v>
@@ -57028,7 +58147,7 @@
         <v>155</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>156</v>
@@ -57039,7 +58158,7 @@
         <v>157</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>158</v>
@@ -57050,7 +58169,7 @@
         <v>159</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>72</v>
@@ -57061,7 +58180,7 @@
         <v>160</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>72</v>
@@ -57072,7 +58191,7 @@
         <v>161</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>162</v>
@@ -57083,7 +58202,7 @@
         <v>163</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>72</v>
@@ -57094,7 +58213,7 @@
         <v>164</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>165</v>
@@ -57105,7 +58224,7 @@
         <v>166</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>167</v>
@@ -57116,7 +58235,7 @@
         <v>168</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>169</v>
@@ -57127,7 +58246,7 @@
         <v>170</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>72</v>
@@ -57138,7 +58257,7 @@
         <v>171</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>72</v>
@@ -57149,7 +58268,7 @@
         <v>172</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>72</v>
@@ -57160,7 +58279,7 @@
         <v>173</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>174</v>
@@ -57171,7 +58290,7 @@
         <v>175</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>176</v>
@@ -57182,7 +58301,7 @@
         <v>177</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>178</v>
@@ -57193,7 +58312,7 @@
         <v>179</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>72</v>
@@ -57204,7 +58323,7 @@
         <v>180</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>181</v>
@@ -57215,7 +58334,7 @@
         <v>182</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>183</v>
@@ -57226,7 +58345,7 @@
         <v>184</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>185</v>
@@ -57237,7 +58356,7 @@
         <v>188</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>189</v>
@@ -57248,7 +58367,7 @@
         <v>190</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>72</v>
@@ -57259,7 +58378,7 @@
         <v>191</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>72</v>
@@ -57270,7 +58389,7 @@
         <v>192</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>193</v>
@@ -57281,7 +58400,7 @@
         <v>194</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>195</v>
@@ -57292,7 +58411,7 @@
         <v>196</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>197</v>
@@ -57303,7 +58422,7 @@
         <v>198</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>199</v>
@@ -57314,7 +58433,7 @@
         <v>200</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>201</v>
@@ -57325,7 +58444,7 @@
         <v>202</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>203</v>
@@ -57336,7 +58455,7 @@
         <v>204</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>205</v>
@@ -57347,7 +58466,7 @@
         <v>207</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>208</v>
@@ -57358,7 +58477,7 @@
         <v>209</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>210</v>
@@ -57369,7 +58488,7 @@
         <v>211</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>72</v>
@@ -57380,7 +58499,7 @@
         <v>212</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>213</v>
@@ -57391,7 +58510,7 @@
         <v>214</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>215</v>
@@ -57402,7 +58521,7 @@
         <v>216</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>72</v>
@@ -57413,7 +58532,7 @@
         <v>217</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>72</v>
@@ -57424,7 +58543,7 @@
         <v>218</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>219</v>
@@ -57435,7 +58554,7 @@
         <v>220</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>221</v>
@@ -57446,7 +58565,7 @@
         <v>222</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>223</v>
@@ -57457,7 +58576,7 @@
         <v>224</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>225</v>
@@ -57468,7 +58587,7 @@
         <v>226</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>72</v>
@@ -57479,7 +58598,7 @@
         <v>227</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>228</v>
@@ -57490,7 +58609,7 @@
         <v>229</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>230</v>
@@ -57501,7 +58620,7 @@
         <v>231</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>232</v>
@@ -57512,7 +58631,7 @@
         <v>233</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>234</v>
@@ -57523,7 +58642,7 @@
         <v>235</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>236</v>
@@ -57534,7 +58653,7 @@
         <v>237</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>238</v>
@@ -57545,7 +58664,7 @@
         <v>239</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>240</v>
@@ -57556,7 +58675,7 @@
         <v>241</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>72</v>
@@ -57567,7 +58686,7 @@
         <v>242</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>243</v>
@@ -57578,7 +58697,7 @@
         <v>244</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>245</v>
@@ -57589,7 +58708,7 @@
         <v>246</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>247</v>
@@ -57609,7 +58728,7 @@
         <v>249</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>72</v>
@@ -57620,7 +58739,7 @@
         <v>250</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>72</v>
@@ -57631,7 +58750,7 @@
         <v>251</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>72</v>
@@ -57642,7 +58761,7 @@
         <v>252</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C163" s="2" t="s">
         <v>72</v>
@@ -57653,7 +58772,7 @@
         <v>253</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>72</v>
@@ -57664,7 +58783,7 @@
         <v>254</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>255</v>
@@ -57675,7 +58794,7 @@
         <v>256</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>72</v>
@@ -57686,7 +58805,7 @@
         <v>257</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C167" s="2" t="s">
         <v>72</v>
@@ -57697,7 +58816,7 @@
         <v>258</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>259</v>
@@ -57708,7 +58827,7 @@
         <v>260</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>72</v>
@@ -57719,7 +58838,7 @@
         <v>261</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>72</v>
@@ -57730,7 +58849,7 @@
         <v>262</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>72</v>
@@ -57741,7 +58860,7 @@
         <v>263</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>264</v>
@@ -57752,7 +58871,7 @@
         <v>265</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>266</v>
@@ -57763,7 +58882,7 @@
         <v>267</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>268</v>
@@ -57774,7 +58893,7 @@
         <v>269</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="176">
@@ -57782,7 +58901,7 @@
         <v>270</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>271</v>
@@ -57793,7 +58912,7 @@
         <v>272</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>72</v>
@@ -57804,7 +58923,7 @@
         <v>273</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C178" s="2" t="s">
         <v>274</v>
@@ -57815,7 +58934,7 @@
         <v>275</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C179" s="2" t="s">
         <v>276</v>
@@ -57826,7 +58945,7 @@
         <v>277</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>278</v>
@@ -57837,7 +58956,7 @@
         <v>279</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C181" s="2" t="s">
         <v>72</v>
@@ -57848,7 +58967,7 @@
         <v>280</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>72</v>
@@ -57859,7 +58978,7 @@
         <v>281</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C183" s="2" t="s">
         <v>282</v>
@@ -57870,7 +58989,7 @@
         <v>283</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>284</v>
@@ -57881,7 +59000,7 @@
         <v>286</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>72</v>
@@ -57892,7 +59011,7 @@
         <v>287</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>72</v>
@@ -57903,7 +59022,7 @@
         <v>288</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>289</v>
@@ -57914,7 +59033,7 @@
         <v>290</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>72</v>
@@ -57925,7 +59044,7 @@
         <v>291</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>292</v>
@@ -57936,7 +59055,7 @@
         <v>293</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C190" s="2" t="s">
         <v>294</v>
@@ -57947,7 +59066,7 @@
         <v>295</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>296</v>
@@ -57958,7 +59077,7 @@
         <v>297</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C192" s="2" t="s">
         <v>298</v>
@@ -57969,7 +59088,7 @@
         <v>299</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C193" s="2" t="s">
         <v>300</v>
@@ -57980,7 +59099,7 @@
         <v>301</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C194" s="2" t="s">
         <v>302</v>
@@ -57991,7 +59110,7 @@
         <v>303</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C195" s="2" t="s">
         <v>304</v>
@@ -58002,7 +59121,7 @@
         <v>305</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C196" s="2" t="s">
         <v>72</v>
@@ -58013,7 +59132,7 @@
         <v>306</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>72</v>
@@ -58024,7 +59143,7 @@
         <v>307</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>308</v>
@@ -58035,7 +59154,7 @@
         <v>311</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>312</v>
@@ -58046,7 +59165,7 @@
         <v>313</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C200" s="2" t="s">
         <v>314</v>
@@ -58057,7 +59176,7 @@
         <v>315</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>3014</v>
+        <v>3111</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>316</v>
@@ -58068,7 +59187,7 @@
         <v>317</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>3013</v>
+        <v>3110</v>
       </c>
       <c r="C202" s="2" t="s">
         <v>318</v>
@@ -60489,16 +61608,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="8" t="s">
-        <v>3010</v>
+        <v>3107</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3015</v>
+        <v>3112</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3016</v>
+        <v>3113</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3012</v>
+        <v>3109</v>
       </c>
     </row>
     <row r="2">

</xml_diff>